<commit_message>
Fix displaying of PR in stock_card_new
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>PROGEN Dieseltech Services Corp.</t>
   </si>
@@ -35,15 +35,21 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2020-01-16</t>
+    <t>2020-08-03</t>
   </si>
   <si>
     <t>Main Category</t>
   </si>
   <si>
+    <t>Electrical, Instrumentation and Control</t>
+  </si>
+  <si>
     <t>Sub-Category</t>
   </si>
   <si>
+    <t>EIC Parts and Accessories</t>
+  </si>
+  <si>
     <t>No.</t>
   </si>
   <si>
@@ -78,27 +84,6 @@
   </si>
   <si>
     <t>Bin</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>CON-HOU_1001</t>
-  </si>
-  <si>
-    <t>Rags, Cotton</t>
-  </si>
-  <si>
-    <t>kg/s</t>
-  </si>
-  <si>
-    <t>PRO-WH-RM1</t>
-  </si>
-  <si>
-    <t>PROGEN</t>
-  </si>
-  <si>
-    <t>SR Cabinet 1-A</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared By: </t>
@@ -236,17 +221,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
@@ -616,7 +595,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C1" sqref="C1"/>
@@ -625,50 +604,50 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="6"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="5"/>
+      <c r="A2" s="3"/>
       <c r="B2"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="3"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="O2"/>
@@ -680,19 +659,19 @@
       <c r="U2"/>
       <c r="V2"/>
       <c r="W2"/>
-      <c r="X2" s="7"/>
+      <c r="X2" s="5"/>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="5"/>
+      <c r="A3" s="3"/>
       <c r="B3"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="3"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
@@ -708,196 +687,143 @@
       <c r="U3"/>
       <c r="V3"/>
       <c r="W3"/>
-      <c r="X3" s="7"/>
+      <c r="X3" s="5"/>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="10"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="8"/>
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
       <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2" t="s">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2" t="s">
+      <c r="M10" s="1"/>
+      <c r="N10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="O10" s="1"/>
+      <c r="P10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2" t="s">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2" t="s">
+      <c r="S10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="T10" s="1"/>
+      <c r="U10" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
+    <row r="13" spans="1:24">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="3">
-        <v>10</v>
-      </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3">
-        <v>50</v>
-      </c>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2" t="s">
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="G13" t="s">
         <v>25</v>
       </c>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1" t="s">
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1" t="s">
+      <c r="D16" t="s">
         <v>27</v>
       </c>
-      <c r="X11" s="1"/>
-    </row>
-    <row r="14" spans="1:24">
-      <c r="A14" t="s">
+      <c r="G16" t="s">
         <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
-    <protectedRange name="p4d5aa7598328d9c23de814036e20b8b5" sqref="A11:X11" password="C724"/>
-    <protectedRange name="p02bab403cdc520e840a32a278a71d195" sqref="A14:X14" password="C724"/>
-    <protectedRange name="pf1cbf82c11b0471a0a61f7a481e7bcdb" sqref="A16:X16" password="C724"/>
+    <protectedRange name="p21e30e0b9d08ee520ad514689fe8f17e" sqref="A13:X13" password="C724"/>
+    <protectedRange name="pdd3015a4fb1570e6634a519c28529b98" sqref="A15:X15" password="C724"/>
   </protectedRanges>
   <mergeCells>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="U11:V11"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:K10"/>

</xml_diff>